<commit_message>
small changes in manuscript figures and tables
</commit_message>
<xml_diff>
--- a/manuscript/tables/clan-table.xlsx
+++ b/manuscript/tables/clan-table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idamei/phd/manuscript/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64AB9B86-2B51-DB46-BE95-F6C797A564E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D89589D-15B3-EE4F-8E04-712A8B601E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{171DD23E-46AE-504D-BDCD-0CA54D12CF71}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
   <si>
     <t>CAZy clan</t>
   </si>
@@ -44,12 +44,6 @@
     <t>CAZy families</t>
   </si>
   <si>
-    <t>X586, X606, X608, X610, X611, X612</t>
-  </si>
-  <si>
-    <t>X605, X607, X609, X613, X614, X615</t>
-  </si>
-  <si>
     <t>Structural subclass Locher</t>
   </si>
   <si>
@@ -59,21 +53,9 @@
     <t>GT-CB1</t>
   </si>
   <si>
-    <t>X571</t>
-  </si>
-  <si>
-    <t>X617</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>GT-CA (7 conserved)</t>
-  </si>
-  <si>
-    <t>GT-CB (10 conserved)</t>
-  </si>
-  <si>
     <t>GT66</t>
   </si>
   <si>
@@ -89,9 +71,6 @@
     <t>GT53</t>
   </si>
   <si>
-    <t>Lipid-P</t>
-  </si>
-  <si>
     <t>GT22</t>
   </si>
   <si>
@@ -120,6 +99,24 @@
   </si>
   <si>
     <t>GT-CB3</t>
+  </si>
+  <si>
+    <t>GT-CA (7 conserved TM helices)</t>
+  </si>
+  <si>
+    <t>GT-CB (10 conserved TM helices)</t>
+  </si>
+  <si>
+    <t>GTxx1</t>
+  </si>
+  <si>
+    <t>GTxx3, GTxx7, GTxx8, GTxx9, GTx10, GTx11</t>
+  </si>
+  <si>
+    <t>GTxx2, GTx12, GTx13, GTx14, GTx15, GTx16, GTx17</t>
+  </si>
+  <si>
+    <t>GTxx4, GTxx5, GTxx6</t>
   </si>
 </sst>
 </file>
@@ -149,7 +146,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -157,13 +154,78 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -480,232 +542,240 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2623CA1E-152F-564F-AC63-B2698A471404}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="43.83203125" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>25</v>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+      <c r="B8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+      <c r="B9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+      <c r="B13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J17" t="s">
-        <v>9</v>
-      </c>
-      <c r="K17" t="s">
-        <v>18</v>
-      </c>
-      <c r="L17" t="s">
-        <v>22</v>
-      </c>
-      <c r="M17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J18" t="s">
-        <v>9</v>
-      </c>
-      <c r="K18" t="s">
+      <c r="D14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="L18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J19" t="s">
-        <v>9</v>
-      </c>
-      <c r="K19" t="s">
-        <v>20</v>
-      </c>
-      <c r="L19" t="s">
-        <v>22</v>
-      </c>
-      <c r="M19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="10:13" x14ac:dyDescent="0.2">
-      <c r="J20" t="s">
-        <v>9</v>
-      </c>
-      <c r="K20" t="s">
-        <v>21</v>
-      </c>
-      <c r="L20" t="s">
-        <v>22</v>
-      </c>
-      <c r="M20" t="s">
-        <v>17</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A10"/>
+  <mergeCells count="3">
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A11:A14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>